<commit_message>
Agent query: Please upload a valid Excel file and check if the entries are processed without any date serialization errors.
</commit_message>
<xml_diff>
--- a/invalid_template.xlsx
+++ b/invalid_template.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,88 +436,140 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>document_id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>date</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>account</t>
-        </is>
-      </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>account_code</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>movement</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>customer_identification</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>branch_office</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>description</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>debit</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>credit</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>reference</t>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>cost_center</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>observations</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>27441</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>2024-01-01</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>1010</t>
-        </is>
-      </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>11050501</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Debit</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>13832081</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>Test debit</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>REF001</t>
+      <c r="H2" t="n">
+        <v>235</v>
+      </c>
+      <c r="I2" t="n">
+        <v>119000</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Observaciones</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>27441</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>2024-01-01</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>11100501</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Credit</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>13832081</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>Test credit</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>500</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>REF002</t>
+      <c r="H3" t="n">
+        <v>235</v>
+      </c>
+      <c r="I3" t="n">
+        <v>90000</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Observaciones</t>
         </is>
       </c>
     </row>

</xml_diff>